<commit_message>
remove old figures folder E
</commit_message>
<xml_diff>
--- a/05. Models/06.Benchmarking/CaseOverview.xlsx
+++ b/05. Models/06.Benchmarking/CaseOverview.xlsx
@@ -87,18 +87,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -119,15 +113,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,7 +404,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,7 +446,7 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="2"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -463,36 +456,40 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="2"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="2"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="2"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="2"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="5"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -501,8 +498,8 @@
       <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="5"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
@@ -511,9 +508,9 @@
       <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>

</xml_diff>

<commit_message>
update case overview and loop script folder E
</commit_message>
<xml_diff>
--- a/05. Models/06.Benchmarking/CaseOverview.xlsx
+++ b/05. Models/06.Benchmarking/CaseOverview.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
   <si>
     <t>Case</t>
   </si>
@@ -42,9 +42,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>ByStages high nb</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -57,13 +54,19 @@
     <t>G</t>
   </si>
   <si>
-    <t>ByStages nc</t>
-  </si>
-  <si>
     <t>Clustering nc</t>
   </si>
   <si>
     <t>Clustering optimal nb</t>
+  </si>
+  <si>
+    <t>ByStages nc (10-250)</t>
+  </si>
+  <si>
+    <t>ByStages high nb (250-4000)</t>
+  </si>
+  <si>
+    <t>Running</t>
   </si>
 </sst>
 </file>
@@ -404,7 +407,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,7 +415,7 @@
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -424,16 +427,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -478,22 +481,26 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -527,12 +534,16 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="E11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -559,12 +570,12 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
@@ -591,7 +602,7 @@
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove unnecessary cases folder D
</commit_message>
<xml_diff>
--- a/05. Models/06.Benchmarking/CaseOverview.xlsx
+++ b/05. Models/06.Benchmarking/CaseOverview.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>Case</t>
   </si>
@@ -66,7 +66,7 @@
     <t>ByStages high nb (250-4000)</t>
   </si>
   <si>
-    <t>Running</t>
+    <t>Done up to 150 (incl)</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,9 +481,7 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -492,10 +490,10 @@
         <v>9</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -537,9 +535,6 @@
         <v>9</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="E11" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">

</xml_diff>

<commit_message>
Update Results folder J IEEE 10-200, L
</commit_message>
<xml_diff>
--- a/05. Models/06.Benchmarking/CaseOverview.xlsx
+++ b/05. Models/06.Benchmarking/CaseOverview.xlsx
@@ -128,7 +128,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,12 +138,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -160,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -169,7 +163,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,9 +706,9 @@
       <c r="E2" s="3"/>
       <c r="F2" s="4"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -725,9 +718,9 @@
       <c r="C3" s="2"/>
       <c r="D3" s="4"/>
       <c r="F3" s="2"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -736,9 +729,10 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="K4" s="6"/>
+      <c r="F4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">

</xml_diff>

<commit_message>
hpc files and case overview
</commit_message>
<xml_diff>
--- a/05. Models/06.Benchmarking/CaseOverview.xlsx
+++ b/05. Models/06.Benchmarking/CaseOverview.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_C9E949A40A075553DC11F6543A106D2331323CE3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF98B054-23B6-4B96-B005-385775EECCDC}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_C9E949A40A075553DC11F6543A106D2331323CE3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4BFA8D3-4C81-4CEC-8AFF-7C65C5A64269}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="28">
   <si>
     <t>Case</t>
   </si>
@@ -170,10 +170,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,7 +492,7 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
@@ -504,7 +504,7 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
+      <c r="A3" s="6"/>
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -514,7 +514,7 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
+      <c r="A4" s="6"/>
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -524,7 +524,7 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
+      <c r="A5" s="6"/>
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -534,7 +534,7 @@
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
+      <c r="A6" s="6"/>
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -546,7 +546,7 @@
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
@@ -558,7 +558,7 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
+      <c r="A8" s="6"/>
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -567,26 +567,26 @@
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
+      <c r="A9" s="6"/>
       <c r="B9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
+      <c r="A10" s="6"/>
       <c r="B10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
+      <c r="A11" s="6"/>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B12" t="s">
@@ -594,31 +594,31 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
+      <c r="A13" s="6"/>
       <c r="B13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
+      <c r="A14" s="6"/>
       <c r="B14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
+      <c r="A15" s="6"/>
       <c r="B15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
+      <c r="A16" s="6"/>
       <c r="B16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B17" t="s">
@@ -626,25 +626,25 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
+      <c r="A18" s="6"/>
       <c r="B18" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
+      <c r="A19" s="6"/>
       <c r="B19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
+      <c r="A20" s="6"/>
       <c r="B20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
+      <c r="A21" s="6"/>
       <c r="B21" t="s">
         <v>9</v>
       </c>
@@ -665,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C7DA4E4-FCA7-4842-9F7C-E8AD515AE353}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -710,11 +710,11 @@
       <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="6"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -726,9 +726,9 @@
       <c r="A3">
         <v>150</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -742,9 +742,9 @@
       <c r="A4">
         <v>200</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -758,9 +758,9 @@
       <c r="A5">
         <v>250</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -774,9 +774,9 @@
       <c r="A6">
         <v>300</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -790,9 +790,9 @@
       <c r="A7">
         <v>350</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -806,9 +806,9 @@
       <c r="A8">
         <v>400</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -825,12 +825,155 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7433458-16CD-46D0-A28C-11002359ED71}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>150</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>200</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>250</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>300</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>350</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>400</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update scripts folder J
</commit_message>
<xml_diff>
--- a/05. Models/06.Benchmarking/CaseOverview.xlsx
+++ b/05. Models/06.Benchmarking/CaseOverview.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="44" documentId="11_C9E949A40A075553DC11F6543A106D2331323CE3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFE6CF7B-69CE-4533-9A85-8CE3509851D6}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="11_C9E949A40A075553DC11F6543A106D2331323CE3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC6BF921-2EC7-4C1E-B8DD-C8E3B26B3B0C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -172,19 +172,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1149,7 +1147,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1194,10 +1192,10 @@
       <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="6"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -1209,10 +1207,10 @@
       <c r="A3">
         <v>150</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1224,10 +1222,10 @@
       <c r="A4">
         <v>200</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>

</xml_diff>

<commit_message>
Visualisations: subplots for multiple cases TSC
</commit_message>
<xml_diff>
--- a/05. Models/06.Benchmarking/CaseOverview.xlsx
+++ b/05. Models/06.Benchmarking/CaseOverview.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="47" documentId="11_C9E949A40A075553DC11F6543A106D2331323CE3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC6BF921-2EC7-4C1E-B8DD-C8E3B26B3B0C}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="11_C9E949A40A075553DC11F6543A106D2331323CE3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{001AB50F-B766-457E-B201-732A3DF53FA0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -172,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -180,6 +180,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -501,7 +502,7 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
@@ -513,7 +514,7 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
+      <c r="A3" s="8"/>
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -523,7 +524,7 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
+      <c r="A4" s="8"/>
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -533,7 +534,7 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -543,7 +544,7 @@
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
+      <c r="A6" s="8"/>
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -555,7 +556,7 @@
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
@@ -567,7 +568,7 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8"/>
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -576,26 +577,26 @@
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8"/>
       <c r="B9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
+      <c r="A10" s="8"/>
       <c r="B10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+      <c r="A11" s="8"/>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B12" t="s">
@@ -603,31 +604,31 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
+      <c r="A13" s="8"/>
       <c r="B13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
+      <c r="A14" s="8"/>
       <c r="B14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
+      <c r="A15" s="8"/>
       <c r="B15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
+      <c r="A16" s="8"/>
       <c r="B16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B17" t="s">
@@ -635,25 +636,25 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
+      <c r="A18" s="8"/>
       <c r="B18" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
+      <c r="A19" s="8"/>
       <c r="B19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
+      <c r="A20" s="8"/>
       <c r="B20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
+      <c r="A21" s="8"/>
       <c r="B21" t="s">
         <v>9</v>
       </c>
@@ -834,10 +835,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7433458-16CD-46D0-A28C-11002359ED71}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:L8"/>
+      <selection activeCell="F9" sqref="F9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -981,6 +982,16 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1144,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1192,16 +1203,16 @@
       <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -1292,6 +1303,13 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>